<commit_message>
feat: handle vue template
</commit_message>
<xml_diff>
--- a/locales.xlsx
+++ b/locales.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="前端keyValue1695803255269.xlsx" sheetId="1" r:id="rId1"/>
+    <sheet name="前端keyValue1696814218288.xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -396,9 +396,25 @@
         <v>en-US</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>ce5b42</v>
+      </c>
+      <c r="B2" t="str">
+        <v>天才/帅哥。。</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>ce5b42-Loading</v>
+      </c>
+      <c r="B3" t="str">
+        <v>加载中...</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: partial reconstruction and optimization
</commit_message>
<xml_diff>
--- a/locales.xlsx
+++ b/locales.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="前端keyValue1696814218288.xlsx" sheetId="1" r:id="rId1"/>
+    <sheet name="前端keyValue1696839541659.xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -404,17 +404,9 @@
         <v>天才/帅哥。。</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>ce5b42-Loading</v>
-      </c>
-      <c r="B3" t="str">
-        <v>加载中...</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: ignore template no chinese
</commit_message>
<xml_diff>
--- a/locales.xlsx
+++ b/locales.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="前端keyValue1696839541659.xlsx" sheetId="1" r:id="rId1"/>
+    <sheet name="前端keyValue1696922844719.xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -398,10 +398,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ce5b42</v>
+        <v>5c8de2</v>
       </c>
       <c r="B2" t="str">
-        <v>天才/帅哥。。</v>
+        <v>选择地址</v>
       </c>
     </row>
   </sheetData>

</xml_diff>